<commit_message>
Update mapping file via Streamlit app
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B541"/>
+  <dimension ref="A1:B542"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4829,6 +4829,14 @@
       </c>
       <c r="B541" t="inlineStr"/>
     </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>Hima</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>